<commit_message>
Update and final execution
</commit_message>
<xml_diff>
--- a/PageObjectModelProject/TestData/AddEmp.xlsx
+++ b/PageObjectModelProject/TestData/AddEmp.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CBDBF73-B81C-4303-B8F0-B928DB4E0F98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45F25AA5-9451-4CD9-B36A-DC2C6BEAED18}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="1425" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddEmp" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>testId</t>
   </si>
@@ -66,16 +66,12 @@
   </si>
   <si>
     <t>TC_Login_003</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,15 +452,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -521,9 +519,6 @@
       <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>